<commit_message>
proposed station distr data added. needs testing
</commit_message>
<xml_diff>
--- a/newnodedistros.xlsx
+++ b/newnodedistros.xlsx
@@ -1,15 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gkbytes/capitalbikeshare/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B970D8E7-F8FF-C14F-B2EF-4ECE5A2F1B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="270" windowWidth="28380" windowHeight="12465"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="24280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="endpriors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -136,16 +153,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="0.00000000000000000%"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,49 +255,41 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -293,6 +298,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -339,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,9 +384,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,6 +436,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -580,1549 +629,1525 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="2" max="5" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
+    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="str">
         <f>F2</f>
         <v>newnode</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="B3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>31104</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>C4</f>
         <v>0.16</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.16</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.44</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f>$J$6*(1-D4/$J$7)</f>
         <v>0.06</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="3">
         <f>(1-E4)*B4</f>
         <v>0.15040000000000001</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>F4</f>
         <v>0.15040000000000001</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>31110</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f>C5-C4</f>
         <v>0.17</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.33</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f t="shared" ref="E5:E9" si="0">$J$6*(1-D5/$J$7)</f>
         <v>0.21000000000000002</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="3">
         <f t="shared" ref="F5:F9" si="1">(1-E5)*B5</f>
         <v>0.1343</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>F5+G4</f>
         <v>0.28470000000000001</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>31113</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f t="shared" ref="B6:B9" si="2">C6-C5</f>
         <v>0.18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.51</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.21000000000000002</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>0.14219999999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" ref="G6:G10" si="3">F6+G5</f>
         <v>0.4269</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>31114</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <f t="shared" si="2"/>
         <v>0.17999999999999994</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.69</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.37</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
         <v>0.15659999999999993</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="3"/>
         <v>0.58349999999999991</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>31116</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <f t="shared" si="2"/>
         <v>0.1100000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.42</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>8.0000000000000016E-2</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>0.10120000000000008</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="3"/>
         <v>0.68469999999999998</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <f t="shared" si="2"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
         <v>0.5</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="3"/>
         <v>0.88469999999999993</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>1000</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="3">
         <f>1-SUM(F4:F9)</f>
         <v>0.11530000000000007</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="E11" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <f>SUM(F4:F10)</f>
         <v>1</v>
       </c>
-      <c r="G11" s="6" t="b">
+      <c r="G11" s="7" t="b">
         <f>1=F11</f>
         <v>1</v>
       </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="str">
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="str">
         <f>F17</f>
         <v>newnode</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickTop="1">
-      <c r="B18" t="s">
+    <row r="18" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <f>A4</f>
         <v>31104</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <f>C19</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <f>D4</f>
         <v>0.44</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f>E4</f>
         <v>0.06</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="3">
         <f>(1-E19)*B19</f>
         <v>0.16449999999999998</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <f>F19</f>
         <v>0.16449999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <f t="shared" ref="A20:A25" si="4">A5</f>
         <v>31110</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <f>C20-C19</f>
         <v>0.22400000000000003</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.39900000000000002</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <f t="shared" ref="D20:E24" si="5">D5</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <f t="shared" si="5"/>
         <v>0.21000000000000002</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="3">
         <f t="shared" ref="F20:F24" si="6">(1-E20)*B20</f>
         <v>0.17696000000000003</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f>F20+G19</f>
         <v>0.34145999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <f t="shared" si="4"/>
         <v>31113</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <f t="shared" ref="B21:B24" si="7">C21-C20</f>
         <v>0.125</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.52400000000000002</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <f t="shared" si="5"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <f t="shared" si="5"/>
         <v>0.21000000000000002</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="3">
         <f t="shared" si="6"/>
         <v>9.8750000000000004E-2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <f t="shared" ref="G21:G25" si="8">F21+G20</f>
         <v>0.44020999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <f t="shared" si="4"/>
         <v>31114</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <f t="shared" si="7"/>
         <v>0.18399999999999994</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <f t="shared" si="5"/>
         <v>0.37</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f t="shared" si="5"/>
         <v>0.13</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="3">
         <f t="shared" si="6"/>
         <v>0.16007999999999994</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <f t="shared" si="8"/>
         <v>0.60028999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <f t="shared" si="4"/>
         <v>31116</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <f t="shared" si="7"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>0.84</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <f t="shared" si="5"/>
         <v>0.42</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f t="shared" si="5"/>
         <v>8.0000000000000016E-2</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="3">
         <f t="shared" si="6"/>
         <v>0.12143999999999999</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <f t="shared" si="8"/>
         <v>0.72172999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="27" t="str">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="str">
         <f t="shared" si="4"/>
         <v>31296 [1]</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <f t="shared" si="7"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="3">
         <f t="shared" si="6"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <f t="shared" si="8"/>
         <v>0.88173000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <f t="shared" si="4"/>
         <v>1000</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="3">
         <f>1-SUM(F19:F24)</f>
         <v>0.11826999999999999</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="F26" s="5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="6">
         <f>SUM(F19:F25)</f>
         <v>1</v>
       </c>
-      <c r="G26" s="6" t="b">
+      <c r="G26" s="7" t="b">
         <f>1=F26</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+    <row r="31" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickTop="1">
-      <c r="B32" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <f>A19</f>
         <v>31104</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <f>C33</f>
         <v>0.186</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>0.186</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="9">
         <f>B33/SUM($B$33:$B$38)*(1-$F$39)</f>
         <v>0.16427798999999998</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <f>F33</f>
         <v>0.16427798999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <f t="shared" ref="A34:A38" si="9">A20</f>
         <v>31110</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <f>C34-C33</f>
         <v>0.254</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>0.44</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="9">
         <f t="shared" ref="F34:F38" si="10">B34/SUM($B$33:$B$38)*(1-$F$39)</f>
         <v>0.22433660999999999</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <f>F34+G33</f>
         <v>0.38861459999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <f t="shared" si="9"/>
         <v>31113</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <f t="shared" ref="B35:B38" si="11">C35-C34</f>
         <v>8.2000000000000017E-2</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>0.52200000000000002</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="9">
         <f t="shared" si="10"/>
         <v>7.2423630000000017E-2</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2">
         <f t="shared" ref="G35:G39" si="12">F35+G34</f>
         <v>0.46103822999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <f t="shared" si="9"/>
         <v>31114</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <f t="shared" si="11"/>
         <v>0.17799999999999994</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>0.7</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="9">
         <f t="shared" si="10"/>
         <v>0.15721226999999993</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <f t="shared" si="12"/>
         <v>0.61825049999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <f t="shared" si="9"/>
         <v>31116</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <f t="shared" si="11"/>
         <v>0.17000000000000004</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>0.87</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="9">
         <f t="shared" si="10"/>
         <v>0.15014655000000002</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2">
         <f t="shared" si="12"/>
         <v>0.76839704999999991</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="27" t="str">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="str">
         <f t="shared" si="9"/>
         <v>31296 [1]</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <f t="shared" si="11"/>
         <v>0.13</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="28">
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
         <f t="shared" si="10"/>
         <v>0.11481795</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <f t="shared" si="12"/>
         <v>0.88321499999999986</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="27" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="9">
         <f>AVERAGE(F25,F10)</f>
         <v>0.11678500000000003</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <f t="shared" si="12"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="F40" s="5">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F40" s="6">
         <f>SUM(F33:F39)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="G40" s="6" t="b">
+      <c r="G40" s="7" t="b">
         <f>1=F40</f>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="A49" s="9" t="s">
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="12">
         <v>31104</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="12">
         <v>31110</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="12">
         <v>31113</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="12">
         <v>31114</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F49" s="12">
         <v>31116</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G49" s="12">
         <v>31296</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H49" s="12">
         <v>1000</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M49" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
-      <c r="A50" s="10">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="12">
         <v>31104</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="13">
         <v>8.9562000000000003E-2</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="13">
         <v>0.25373200000000001</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="13">
         <v>8.9552000000000007E-2</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="13">
         <v>0.19900499999999999</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="13">
         <v>0.23383100000000001</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="13">
         <v>0.134328</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <f ca="1">IF(I50&lt;M50,J50+((K50-J50)*(L50-J50)*I50)^0.5,K50-((K50-J50)*(K50-L50)*(1-I50))^0.5)</f>
-        <v>0.12988152043386159</v>
-      </c>
-      <c r="I50">
+        <v>0.16409528274784235</v>
+      </c>
+      <c r="I50" s="2">
         <f ca="1">RAND()</f>
-        <v>0.12068008531301588</v>
-      </c>
-      <c r="J50" s="12">
+        <v>0.41229353201995267</v>
+      </c>
+      <c r="J50" s="2">
         <f>MIN(B50:G50)</f>
         <v>8.9552000000000007E-2</v>
       </c>
-      <c r="K50" s="12">
+      <c r="K50" s="2">
         <f>MAX(B50:G50)</f>
         <v>0.25373200000000001</v>
       </c>
-      <c r="L50" s="12">
+      <c r="L50" s="2">
         <f>AVERAGE(J50:K50)</f>
         <v>0.17164200000000002</v>
       </c>
-      <c r="M50" s="12">
+      <c r="M50" s="2">
         <f>(L50-J50)/(K50-J50)</f>
         <v>0.50000000000000011</v>
       </c>
-      <c r="N50" s="13"/>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51" s="10">
+      <c r="N50" s="14"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="12">
         <v>31110</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="13">
         <v>0.14285700000000001</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="13">
         <v>0.13364100000000001</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="13">
         <v>8.2948999999999995E-2</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="13">
         <v>0.26728099999999999</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="13">
         <v>0.11981600000000001</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="13">
         <v>0.25345600000000001</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <f t="shared" ref="H51:H55" ca="1" si="13">IF(I51&lt;M51,J51+((K51-J51)*(L51-J51)*I51)^0.5,K51-((K51-J51)*(K51-L51)*(1-I51))^0.5)</f>
-        <v>0.21294691607117922</v>
-      </c>
-      <c r="I51">
+        <v>0.10198264501899203</v>
+      </c>
+      <c r="I51" s="2">
         <f t="shared" ref="I51:I55" ca="1" si="14">RAND()</f>
-        <v>0.82623063112000583</v>
-      </c>
-      <c r="J51" s="12">
+        <v>2.1324185706170784E-2</v>
+      </c>
+      <c r="J51" s="2">
         <f t="shared" ref="J51:J55" si="15">MIN(B51:G51)</f>
         <v>8.2948999999999995E-2</v>
       </c>
-      <c r="K51" s="12">
+      <c r="K51" s="2">
         <f t="shared" ref="K51:K55" si="16">MAX(B51:G51)</f>
         <v>0.26728099999999999</v>
       </c>
-      <c r="L51" s="12">
+      <c r="L51" s="2">
         <f t="shared" ref="L51:L55" si="17">AVERAGE(J51:K51)</f>
         <v>0.17511499999999999</v>
       </c>
-      <c r="M51" s="12">
+      <c r="M51" s="2">
         <f t="shared" ref="M51:M55" si="18">(L51-J51)/(K51-J51)</f>
         <v>0.5</v>
       </c>
-      <c r="N51" s="12"/>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="10">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="12">
         <v>31113</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="13">
         <v>6.6986000000000004E-2</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="13">
         <v>0.32057400000000003</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="13">
         <v>0.100478</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="13">
         <v>0.15789500000000001</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="13">
         <v>0.143541</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="13">
         <v>0.21052599999999999</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>8.6003071322454536E-2</v>
-      </c>
-      <c r="I52">
+        <v>0.1989080851646281</v>
+      </c>
+      <c r="I52" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1.1247600159292936E-2</v>
-      </c>
-      <c r="J52" s="12">
+        <v>0.53962635808869197</v>
+      </c>
+      <c r="J52" s="2">
         <f t="shared" si="15"/>
         <v>6.6986000000000004E-2</v>
       </c>
-      <c r="K52" s="12">
+      <c r="K52" s="2">
         <f t="shared" si="16"/>
         <v>0.32057400000000003</v>
       </c>
-      <c r="L52" s="12">
+      <c r="L52" s="2">
         <f t="shared" si="17"/>
         <v>0.19378000000000001</v>
       </c>
-      <c r="M52" s="12">
+      <c r="M52" s="2">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="N52" s="12"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="10">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="12">
         <v>31114</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="13">
         <v>0.20535700000000001</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="13">
         <v>0.37946400000000002</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="13">
         <v>4.9106999999999998E-2</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="13">
         <v>0.10267900000000001</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="13">
         <v>4.4643000000000002E-2</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="13">
         <v>0.21875</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0.25599520646260138</v>
-      </c>
-      <c r="I53">
+        <v>0.1367121936782249</v>
+      </c>
+      <c r="I53" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72803123675842318</v>
-      </c>
-      <c r="J53" s="12">
+        <v>0.15122837890925434</v>
+      </c>
+      <c r="J53" s="2">
         <f t="shared" si="15"/>
         <v>4.4643000000000002E-2</v>
       </c>
-      <c r="K53" s="12">
+      <c r="K53" s="2">
         <f t="shared" si="16"/>
         <v>0.37946400000000002</v>
       </c>
-      <c r="L53" s="12">
+      <c r="L53" s="2">
         <f t="shared" si="17"/>
         <v>0.21205350000000001</v>
       </c>
-      <c r="M53" s="12">
+      <c r="M53" s="2">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="N53" s="12"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="10">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" s="12">
         <v>31116</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="13">
         <v>0.23188400000000001</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="13">
         <v>0.23913000000000001</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="13">
         <v>0.108696</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="13">
         <v>0.101449</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="13">
         <v>8.6957000000000007E-2</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G54" s="13">
         <v>0.23188400000000001</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0.13194509633991225</v>
-      </c>
-      <c r="I54">
+        <v>0.20075834954432453</v>
+      </c>
+      <c r="I54" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.17480345954558896</v>
-      </c>
-      <c r="J54" s="12">
+        <v>0.87283261235537879</v>
+      </c>
+      <c r="J54" s="2">
         <f t="shared" si="15"/>
         <v>8.6957000000000007E-2</v>
       </c>
-      <c r="K54" s="12">
+      <c r="K54" s="2">
         <f t="shared" si="16"/>
         <v>0.23913000000000001</v>
       </c>
-      <c r="L54" s="12">
+      <c r="L54" s="2">
         <f t="shared" si="17"/>
         <v>0.16304350000000001</v>
       </c>
-      <c r="M54" s="12">
+      <c r="M54" s="2">
         <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="N54" s="12"/>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" s="10">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="12">
         <v>31296</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="13">
         <v>0.11788700000000001</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="13">
         <v>0.26441999999999999</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="13">
         <v>0.191057</v>
       </c>
-      <c r="E55" s="11">
+      <c r="E55" s="13">
         <v>0.18699199999999999</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="13">
         <v>0.138211</v>
       </c>
-      <c r="G55" s="11">
+      <c r="G55" s="13">
         <v>0.101525</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0.23766914412476917</v>
-      </c>
-      <c r="I55">
+        <v>0.22283966636685662</v>
+      </c>
+      <c r="I55" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.94606261951940329</v>
-      </c>
-      <c r="J55" s="12">
+        <v>0.86968619462775354</v>
+      </c>
+      <c r="J55" s="2">
         <f t="shared" si="15"/>
         <v>0.101525</v>
       </c>
-      <c r="K55" s="12">
+      <c r="K55" s="2">
         <f t="shared" si="16"/>
         <v>0.26441999999999999</v>
       </c>
-      <c r="L55" s="12">
+      <c r="L55" s="2">
         <f t="shared" si="17"/>
         <v>0.18297249999999998</v>
       </c>
-      <c r="M55" s="12">
+      <c r="M55" s="2">
         <f t="shared" si="18"/>
         <v>0.49999999999999989</v>
       </c>
-      <c r="N55" s="12"/>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="10">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="12">
         <v>1000</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <f ca="1">OFFSET($H$49,B57,0)*(OFFSET($F$3,B57,0)/$F$10)</f>
-        <v>0.16942047418259126</v>
-      </c>
-      <c r="C56">
+        <v>0.21404970099978732</v>
+      </c>
+      <c r="C56" s="2">
         <f ca="1">OFFSET($H$49,C57,0)*(OFFSET($F$3,C57,0)/$F$10)</f>
-        <v>0.24803790831187641</v>
-      </c>
-      <c r="D56">
+        <v>0.11878811124068188</v>
+      </c>
+      <c r="D56" s="2">
         <f t="shared" ref="D56:G56" ca="1" si="19">OFFSET($H$49,D57,0)*(OFFSET($F$3,D57,0)/$F$10)</f>
-        <v>0.10606796827452754</v>
-      </c>
-      <c r="E56">
+        <v>0.24531422125247263</v>
+      </c>
+      <c r="E56" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>0.34769166810098295</v>
-      </c>
-      <c r="F56">
+        <v>0.18568195602784041</v>
+      </c>
+      <c r="F56" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>0.11580957284994903</v>
-      </c>
-      <c r="G56">
+        <v>0.17620767540230395</v>
+      </c>
+      <c r="G56" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>0.41226217541156801</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="10" t="s">
+        <v>0.38653888355048815</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="14">
-        <v>1</v>
-      </c>
-      <c r="C57" s="15">
+      <c r="B57" s="15">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
         <f>1+B57</f>
         <v>2</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="2">
         <f t="shared" ref="D57:G57" si="20">1+C57</f>
         <v>3</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="2">
         <f t="shared" si="20"/>
         <v>4</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="2">
         <f t="shared" si="20"/>
         <v>5</v>
       </c>
-      <c r="G57" s="15">
+      <c r="G57" s="2">
         <f t="shared" si="20"/>
         <v>6</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
-      <c r="B59" s="12"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="K60" t="s">
+      <c r="K60" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="12">
         <v>31104</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="12">
         <v>31110</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="12">
         <v>31113</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="12">
         <v>31114</v>
       </c>
-      <c r="F61" s="10">
+      <c r="F61" s="12">
         <v>31116</v>
       </c>
-      <c r="G61" s="10">
+      <c r="G61" s="12">
         <v>31296</v>
       </c>
-      <c r="H61" s="10">
+      <c r="H61" s="12">
         <v>1000</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
-      <c r="A62" s="10">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="12">
         <v>31104</v>
       </c>
-      <c r="B62" s="22">
+      <c r="B62" s="16">
         <f ca="1">B50/SUM($B50:$G50)*(1-$H50)</f>
-        <v>7.7928771979182687E-2</v>
-      </c>
-      <c r="C62" s="22">
+        <v>7.4864549641041334E-2</v>
+      </c>
+      <c r="C62" s="16">
         <f t="shared" ref="C62:G62" ca="1" si="21">C50/SUM($B50:$G50)*(1-$H50)</f>
-        <v>0.22077469431033234</v>
-      </c>
-      <c r="D62" s="22">
+        <v>0.21209365478127665</v>
+      </c>
+      <c r="D62" s="16">
         <f t="shared" ca="1" si="21"/>
-        <v>7.7920070881398004E-2</v>
-      </c>
-      <c r="E62" s="22">
+        <v>7.485619067745844E-2</v>
+      </c>
+      <c r="E62" s="16">
         <f t="shared" ca="1" si="21"/>
-        <v>0.17315619646409472</v>
-      </c>
-      <c r="F62" s="22">
+        <v>0.16634755478121779</v>
+      </c>
+      <c r="F62" s="16">
         <f t="shared" ca="1" si="21"/>
-        <v>0.20345863960903363</v>
-      </c>
-      <c r="G62" s="22">
+        <v>0.19545848135497573</v>
+      </c>
+      <c r="G62" s="16">
         <f t="shared" ca="1" si="21"/>
-        <v>0.11688010632209701</v>
-      </c>
-      <c r="H62" s="24">
+        <v>0.11228428601618767</v>
+      </c>
+      <c r="H62" s="17">
         <f ca="1">H50</f>
-        <v>0.12988152043386159</v>
-      </c>
-      <c r="I62" s="12">
+        <v>0.16409528274784235</v>
+      </c>
+      <c r="I62" s="2">
         <f ca="1">SUM(B62:H62)</f>
         <v>1</v>
       </c>
-      <c r="J62" t="b">
+      <c r="J62" s="2" t="b">
         <f ca="1">I62=1</f>
         <v>1</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K62" s="2">
         <f>F4</f>
         <v>0.15040000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
-      <c r="A63" s="10">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="12">
         <v>31110</v>
       </c>
-      <c r="B63" s="22">
+      <c r="B63" s="16">
         <f t="shared" ref="B63:G67" ca="1" si="22">B51/SUM($B51:$G51)*(1-$H51)</f>
-        <v>0.11243604241081956</v>
-      </c>
-      <c r="C63" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.10518256118933154</v>
-      </c>
-      <c r="D63" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>6.5285266258811744E-2</v>
-      </c>
-      <c r="E63" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.21036433532557913</v>
-      </c>
-      <c r="F63" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>9.4301552304015601E-2</v>
-      </c>
-      <c r="G63" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.1994833264402632</v>
-      </c>
-      <c r="H63" s="24">
+        <v>0.12828806528052186</v>
+      </c>
+      <c r="C63" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.1200119373370169</v>
+      </c>
+      <c r="D63" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>7.4489641578319624E-2</v>
+      </c>
+      <c r="E63" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.24002297665667879</v>
+      </c>
+      <c r="F63" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.10759684740440446</v>
+      </c>
+      <c r="G63" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.22760788672406637</v>
+      </c>
+      <c r="H63" s="17">
         <f t="shared" ref="H63:H67" ca="1" si="23">H51</f>
-        <v>0.21294691607117922</v>
-      </c>
-      <c r="I63" s="12">
+        <v>0.10198264501899203</v>
+      </c>
+      <c r="I63" s="2">
         <f t="shared" ref="I63:I68" ca="1" si="24">SUM(B63:H63)</f>
         <v>1</v>
       </c>
-      <c r="J63" t="b">
+      <c r="J63" s="2" t="b">
         <f t="shared" ref="J63:J68" ca="1" si="25">I63=1</f>
         <v>1</v>
       </c>
-      <c r="K63" s="3">
+      <c r="K63" s="2">
         <f t="shared" ref="K63:K68" si="26">F5</f>
         <v>0.1343</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
-      <c r="A64" s="10">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="12">
         <v>31113</v>
       </c>
-      <c r="B64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>6.1224998264394065E-2</v>
-      </c>
-      <c r="C64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.29300365141387547</v>
-      </c>
-      <c r="D64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>9.1836583399662414E-2</v>
-      </c>
-      <c r="E64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.14431554505354105</v>
-      </c>
-      <c r="F64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.13119603313930356</v>
-      </c>
-      <c r="G64" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.19242011740676893</v>
-      </c>
-      <c r="H64" s="24">
+      <c r="B64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>5.3661943007162226E-2</v>
+      </c>
+      <c r="C64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.25680923950643453</v>
+      </c>
+      <c r="D64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>8.049211341882849E-2</v>
+      </c>
+      <c r="E64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.12648840789293106</v>
+      </c>
+      <c r="F64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.11498953454738411</v>
+      </c>
+      <c r="G64" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.16865067646263149</v>
+      </c>
+      <c r="H64" s="17">
         <f t="shared" ca="1" si="23"/>
-        <v>8.6003071322454536E-2</v>
-      </c>
-      <c r="I64" s="12">
+        <v>0.1989080851646281</v>
+      </c>
+      <c r="I64" s="2">
         <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
-      <c r="J64" t="b">
+      <c r="J64" s="2" t="b">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="K64" s="3">
+      <c r="K64" s="2">
         <f t="shared" si="26"/>
         <v>0.14219999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
-      <c r="A65" s="10">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="12">
         <v>31114</v>
       </c>
-      <c r="B65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.15278659238645956</v>
-      </c>
-      <c r="C65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.28232303497487543</v>
-      </c>
-      <c r="D65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>3.6535843396241031E-2</v>
-      </c>
-      <c r="E65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>7.6393668195626555E-2</v>
-      </c>
-      <c r="F65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>3.3214605997890084E-2</v>
-      </c>
-      <c r="G65" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.16275104858630593</v>
-      </c>
-      <c r="H65" s="24">
+      <c r="B65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.17728219404282078</v>
+      </c>
+      <c r="C65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.32758664413808608</v>
+      </c>
+      <c r="D65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>4.2393474305043408E-2</v>
+      </c>
+      <c r="E65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>8.8641528665313551E-2</v>
+      </c>
+      <c r="F65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>3.8539757537623003E-2</v>
+      </c>
+      <c r="G65" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.18884420763288828</v>
+      </c>
+      <c r="H65" s="17">
         <f t="shared" ca="1" si="23"/>
-        <v>0.25599520646260138</v>
-      </c>
-      <c r="I65" s="12">
+        <v>0.1367121936782249</v>
+      </c>
+      <c r="I65" s="2">
         <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
-      <c r="J65" t="b">
+      <c r="J65" s="2" t="b">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="K65" s="3">
+      <c r="K65" s="2">
         <f t="shared" si="26"/>
         <v>0.15659999999999993</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="10">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="12">
         <v>31116</v>
       </c>
-      <c r="B66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.2012880432803158</v>
-      </c>
-      <c r="C66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.2075779691122368</v>
-      </c>
-      <c r="D66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>9.4354095808236893E-2</v>
-      </c>
-      <c r="E66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>8.8063301921412235E-2</v>
-      </c>
-      <c r="F66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>7.548345025757025E-2</v>
-      </c>
-      <c r="G66" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.2012880432803158</v>
-      </c>
-      <c r="H66" s="24">
+      <c r="B66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.18533135087426383</v>
+      </c>
+      <c r="C66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.19112265587346566</v>
+      </c>
+      <c r="D66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>8.6874370437930101E-2</v>
+      </c>
+      <c r="E66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>8.1082266197077812E-2</v>
+      </c>
+      <c r="F66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>6.9499656198674167E-2</v>
+      </c>
+      <c r="G66" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.18533135087426383</v>
+      </c>
+      <c r="H66" s="17">
         <f t="shared" ca="1" si="23"/>
-        <v>0.13194509633991225</v>
-      </c>
-      <c r="I66" s="12">
+        <v>0.20075834954432453</v>
+      </c>
+      <c r="I66" s="2">
         <f t="shared" ca="1" si="24"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="J66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" s="2" t="b">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="K66" s="3">
+      <c r="K66" s="2">
         <f t="shared" si="26"/>
         <v>0.10120000000000008</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="10">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="12">
         <v>31296</v>
       </c>
-      <c r="B67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>8.9860630428563917E-2</v>
-      </c>
-      <c r="C67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.20155698166821506</v>
-      </c>
-      <c r="D67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.1456352478881483</v>
-      </c>
-      <c r="E67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.14253665802928248</v>
-      </c>
-      <c r="F67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>0.10535281746216502</v>
-      </c>
-      <c r="G67" s="22">
-        <f t="shared" ca="1" si="22"/>
-        <v>7.7388520398856131E-2</v>
-      </c>
-      <c r="H67" s="24">
+      <c r="B67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>9.160867225316309E-2</v>
+      </c>
+      <c r="C67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.20547783145878157</v>
+      </c>
+      <c r="D67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.14846826278277148</v>
+      </c>
+      <c r="E67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.14530939664223766</v>
+      </c>
+      <c r="F67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.10740222586699062</v>
+      </c>
+      <c r="G67" s="16">
+        <f t="shared" ca="1" si="22"/>
+        <v>7.8893944629199006E-2</v>
+      </c>
+      <c r="H67" s="17">
         <f t="shared" ca="1" si="23"/>
-        <v>0.23766914412476917</v>
-      </c>
-      <c r="I67" s="12">
+        <v>0.22283966636685662</v>
+      </c>
+      <c r="I67" s="2">
         <f t="shared" ca="1" si="24"/>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="J67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" s="2" t="b">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="K67" s="3">
+      <c r="K67" s="2">
         <f t="shared" si="26"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="10">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="12">
         <v>1000</v>
       </c>
-      <c r="B68" s="22">
+      <c r="B68" s="16">
         <f ca="1">OFFSET($H$61,B57,0)*$B$72</f>
-        <v>0.10520403155142789</v>
-      </c>
-      <c r="C68" s="22">
+        <v>0.13291717902575231</v>
+      </c>
+      <c r="C68" s="16">
         <f t="shared" ref="C68:G68" ca="1" si="27">OFFSET($H$61,C57,0)*$B$72</f>
-        <v>0.17248700201765518</v>
-      </c>
-      <c r="D68" s="22">
+        <v>8.2605942465383553E-2</v>
+      </c>
+      <c r="D68" s="16">
         <f t="shared" ca="1" si="27"/>
-        <v>6.9662487771188178E-2</v>
-      </c>
-      <c r="E68" s="22">
+        <v>0.16111554898334876</v>
+      </c>
+      <c r="E68" s="16">
         <f t="shared" ca="1" si="27"/>
-        <v>0.20735611723470712</v>
-      </c>
-      <c r="F68" s="22">
+        <v>0.11073687687936218</v>
+      </c>
+      <c r="F68" s="16">
         <f t="shared" ca="1" si="27"/>
-        <v>0.10687552803532893</v>
-      </c>
-      <c r="G68" s="22">
+        <v>0.16261426313090288</v>
+      </c>
+      <c r="G68" s="16">
         <f t="shared" ca="1" si="27"/>
-        <v>0.19251200674106303</v>
-      </c>
-      <c r="H68" s="25">
+        <v>0.18050012975715388</v>
+      </c>
+      <c r="H68" s="18">
         <f ca="1">1-SUM(B68:G68)</f>
-        <v>0.14590282664862964</v>
-      </c>
-      <c r="I68" s="12">
+        <v>0.16951005975809641</v>
+      </c>
+      <c r="I68" s="2">
         <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
-      <c r="J68" t="b">
+      <c r="J68" s="2" t="b">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="K68" s="3">
+      <c r="K68" s="2">
         <f t="shared" si="26"/>
         <v>0.11530000000000007</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
-      <c r="K69" s="26">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K69" s="19">
         <f>SUM(K62:K68)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
-      <c r="A70" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="20">
         <f ca="1">SUMPRODUCT(B62:B68,$K$62:$K$68)</f>
-        <v>0.10992572382591893</v>
-      </c>
-      <c r="C70" s="2">
+        <v>0.1162844532166883</v>
+      </c>
+      <c r="C70" s="20">
         <f t="shared" ref="C70:H70" ca="1" si="28">SUMPRODUCT(C62:C68,$K$62:$K$68)</f>
-        <v>0.21441347664055682</v>
-      </c>
-      <c r="D70" s="2">
+        <v>0.20579647542571444</v>
+      </c>
+      <c r="D70" s="20">
         <f t="shared" ca="1" si="28"/>
-        <v>8.5975434067845247E-2</v>
-      </c>
-      <c r="E70" s="2">
+        <v>9.6409088188838227E-2</v>
+      </c>
+      <c r="E70" s="20">
         <f t="shared" ca="1" si="28"/>
-        <v>0.14810703920593893</v>
-      </c>
-      <c r="F70" s="2">
+        <v>0.1391570395672323</v>
+      </c>
+      <c r="F70" s="20">
         <f t="shared" ca="1" si="28"/>
-        <v>0.10815459812427905</v>
-      </c>
-      <c r="G70" s="2">
+        <v>0.11349728496492671</v>
+      </c>
+      <c r="G70" s="20">
         <f t="shared" ca="1" si="28"/>
-        <v>0.15526302207261256</v>
-      </c>
-      <c r="H70" s="2">
+        <v>0.15635641150748839</v>
+      </c>
+      <c r="H70" s="20">
         <f t="shared" ca="1" si="28"/>
-        <v>0.17816070606284851</v>
-      </c>
-      <c r="I70" s="3">
+        <v>0.17249924712911174</v>
+      </c>
+      <c r="I70" s="2">
         <f ca="1">SUM(B70:H70)</f>
         <v>1</v>
       </c>
-      <c r="J70" s="3" t="b">
+      <c r="J70" s="2" t="b">
         <f ca="1">1=I70</f>
         <v>1</v>
       </c>
-      <c r="L70" s="16"/>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="A72" t="s">
+      <c r="L70" s="21"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="17">
+      <c r="B72" s="4">
         <v>0.81</v>
       </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="19"/>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="K73" s="20"/>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="16" t="s">
+      <c r="J72" s="14"/>
+      <c r="K72" s="20"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G74" s="15"/>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="G75" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>